<commit_message>
Modulo 6 completo sin ejercicios
</commit_message>
<xml_diff>
--- a/bases/tabla11.xlsx
+++ b/bases/tabla11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irwin\Documents\GitHub\intro_r_ciencias\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B3E0AD-9828-45A0-8E48-F188CC5CCC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E79634-BAD3-4420-BA37-5CFEEB94EFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{18658454-743C-4875-BFC6-167C3F721735}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{18658454-743C-4875-BFC6-167C3F721735}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
     <t>Idéntica a `summarise_all()` es considerada obsoleta (deprecated).</t>
   </si>
   <si>
-    <t>Algunas funciones tienes variantes escritas con "\_" al final o con la palabra summarize (con z). hacen lo mismo que las originales sin "\_" o con summarise (con s).</t>
+    <t>Algunas funciones tienes variantes escritas con "\_" al final o con la palabra summarize (con z), hacen lo mismo que las originales sin "\_" o con summarise (con s).</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>